<commit_message>
add WMA format, package updates
</commit_message>
<xml_diff>
--- a/data/output/~media_report.xlsx
+++ b/data/output/~media_report.xlsx
@@ -7,19 +7,19 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="C_music_library_parser" sheetId="1" r:id="rId1"/>
-    <sheet name="C_music_library_parser_dir" sheetId="2" r:id="rId2"/>
+    <sheet name="music_library-data-input" sheetId="1" r:id="rId1"/>
+    <sheet name="music_library-data-input_dir" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'C_music_library_parser'!$A$1:$Y$65536</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'C_music_library_parser_dir'!$A$1:$E$65536</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'music_library-data-input'!$A$1:$Y$65536</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'music_library-data-input_dir'!$A$1:$E$65536</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="172">
   <si>
     <t>index:</t>
   </si>
@@ -120,9 +120,6 @@
     <t>ALBUM_ART</t>
   </si>
   <si>
-    <t>2013</t>
-  </si>
-  <si>
     <t>4-star</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>INCONSISTENT_GENRE</t>
   </si>
   <si>
-    <t>1991</t>
-  </si>
-  <si>
     <t>2-1/2-star</t>
   </si>
   <si>
@@ -198,9 +192,6 @@
     <t>Post-Punk-Revival</t>
   </si>
   <si>
-    <t>2002</t>
-  </si>
-  <si>
     <t>iTunes v7.6.2.9</t>
   </si>
   <si>
@@ -228,9 +219,6 @@
     <t>Classical</t>
   </si>
   <si>
-    <t>2006</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
@@ -276,9 +264,6 @@
     <t>MISSING_ART</t>
   </si>
   <si>
-    <t>2009</t>
-  </si>
-  <si>
     <t>iTunes 8.1.0.52, QuickTime 7.6</t>
   </si>
   <si>
@@ -309,9 +294,6 @@
     <t>Trip-Hop</t>
   </si>
   <si>
-    <t>2003</t>
-  </si>
-  <si>
     <t>iTunes 9.0.2.25, QuickTime 7.6.5</t>
   </si>
   <si>
@@ -339,9 +321,6 @@
     <t>0:04:55</t>
   </si>
   <si>
-    <t>1993</t>
-  </si>
-  <si>
     <t>iTunes 9.0.3.15, QuickTime 7.6.5</t>
   </si>
   <si>
@@ -369,9 +348,6 @@
     <t>0:02:09</t>
   </si>
   <si>
-    <t>1963</t>
-  </si>
-  <si>
     <t>iTunes 8.0.1.11, QuickTime 7.5.5</t>
   </si>
   <si>
@@ -405,9 +381,6 @@
     <t>0:03:53</t>
   </si>
   <si>
-    <t>1988</t>
-  </si>
-  <si>
     <t>3-1/2-star</t>
   </si>
   <si>
@@ -444,7 +417,7 @@
     <t>Icelandic</t>
   </si>
   <si>
-    <t>1 - Human Behaviour - Björk.flac</t>
+    <t>01~Human Behaviour~Björk~Debut~1993.flac</t>
   </si>
   <si>
     <t>ISO-8859-1</t>
@@ -471,18 +444,48 @@
     <t>Rockabilly</t>
   </si>
   <si>
-    <t>2004</t>
-  </si>
-  <si>
     <t>classic</t>
   </si>
   <si>
-    <t>01~Walkin' After Midnight~Definitive Collection~Patsy Cline~2004.flac</t>
+    <t>01~Walkin' After Midnight~Patsy Cline~Definitive Collection~2004.flac</t>
   </si>
   <si>
     <t>F2CB6F6AF35B1833FC3D2147F1E2473A20C6F7E9CBA89165462D1507C63388C9</t>
   </si>
   <si>
+    <t>07.12 MiB</t>
+  </si>
+  <si>
+    <t>.wma</t>
+  </si>
+  <si>
+    <t>Sallie Ford &amp; The Sound Outside</t>
+  </si>
+  <si>
+    <t>Dirty Radio</t>
+  </si>
+  <si>
+    <t>I Swear</t>
+  </si>
+  <si>
+    <t>0:03:04</t>
+  </si>
+  <si>
+    <t>5-star</t>
+  </si>
+  <si>
+    <t>MediaMonkey 4.1.27</t>
+  </si>
+  <si>
+    <t>Sallie Ford</t>
+  </si>
+  <si>
+    <t>01~I Swear~Sallie Ford &amp; The Sound Outside~Dirty Radio~2011.wma</t>
+  </si>
+  <si>
+    <t>EC54C37EC80A663F04B63428B9BE09BA6FDEF2C912760AB6713D9E5763279151</t>
+  </si>
+  <si>
     <t>Index:</t>
   </si>
   <si>
@@ -529,6 +532,9 @@
   </si>
   <si>
     <t>data\input\Rimsky-Korsakov~Capriccio Espagnol~MP3</t>
+  </si>
+  <si>
+    <t>data\input\Sallie Ford &amp; The Sound Outside ~ Dirty Radio ~ WMA</t>
   </si>
 </sst>
 </file>
@@ -922,7 +928,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -935,7 +941,7 @@
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" customWidth="1"/>
     <col min="6" max="6" width="38.7109375" customWidth="1"/>
     <col min="7" max="7" width="46.7109375" customWidth="1"/>
     <col min="8" max="8" width="6.7109375" customWidth="1"/>
@@ -1072,21 +1078,21 @@
       <c r="L2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="2">
+        <v>2013</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S2" s="6">
         <v>-7.99</v>
@@ -1095,19 +1101,19 @@
         <v>-8.81</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V2" s="2">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="W2" s="7">
         <v>43932.85918427083</v>
       </c>
       <c r="X2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1118,46 +1124,46 @@
         <v>7176192</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="H3" s="2">
         <v>7</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="2">
+        <v>1991</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="P3" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
@@ -1168,19 +1174,19 @@
         <v>-4.34</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="V3" s="2">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="W3" s="7">
         <v>43876.70424291667</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1191,28 +1197,28 @@
         <v>10332160</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="H4" s="2">
         <v>2</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>31</v>
@@ -1220,14 +1226,14 @@
       <c r="L4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>59</v>
+      <c r="M4" s="2">
+        <v>2002</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -1239,19 +1245,19 @@
         <v>-8.470000000000001</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="V4" s="2">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="W4" s="7">
         <v>43876.70372451389</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1262,28 +1268,28 @@
         <v>1814528</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H5" s="2">
         <v>1</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>31</v>
@@ -1291,23 +1297,23 @@
       <c r="L5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="2">
+        <v>2006</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R5" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="S5" s="6">
         <v>-3.61</v>
@@ -1316,19 +1322,19 @@
         <v>-2.5</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="V5" s="2">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="W5" s="7">
         <v>43932.85872113426</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1339,50 +1345,50 @@
         <v>6770846</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="M6" s="2">
+        <v>2009</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="S6" s="6">
         <v>-4.8</v>
@@ -1391,19 +1397,19 @@
         <v>-7.19</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="V6" s="2">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="W6" s="7">
         <v>43932.85997417824</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1414,28 +1420,28 @@
         <v>13749215</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>31</v>
@@ -1443,17 +1449,17 @@
       <c r="L7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>96</v>
+      <c r="M7" s="2">
+        <v>2003</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
@@ -1464,19 +1470,19 @@
         <v>-4.8</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="V7" s="2">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="W7" s="7">
         <v>43876.70344572917</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1487,25 +1493,25 @@
         <v>12461636</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H8" s="2">
         <v>1</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>30</v>
@@ -1516,17 +1522,17 @@
       <c r="L8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>106</v>
+      <c r="M8" s="2">
+        <v>1993</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
@@ -1537,19 +1543,19 @@
         <v>-4.32</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="V8" s="2">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="W8" s="7">
         <v>43876.70200997685</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y8" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1560,49 +1566,49 @@
         <v>5289728</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H9" s="2">
         <v>2</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>116</v>
+        <v>80</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1963</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="R9" s="3"/>
       <c r="S9" s="6">
@@ -1612,19 +1618,19 @@
         <v>-1.36</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="V9" s="2">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="W9" s="7">
         <v>43876.78738667824</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1635,28 +1641,28 @@
         <v>16334985</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="H10" s="2">
         <v>2</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>31</v>
@@ -1664,20 +1670,20 @@
       <c r="L10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>128</v>
+      <c r="M10" s="2">
+        <v>1988</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="R10" s="3"/>
       <c r="S10" s="6">
@@ -1687,19 +1693,19 @@
         <v>0.1</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="V10" s="2">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="W10" s="7">
         <v>43876.70605457176</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1710,43 +1716,43 @@
         <v>24794419</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="H11" s="2">
         <v>1</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="2" t="s">
-        <v>106</v>
+      <c r="M11" s="2">
+        <v>1993</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -1758,19 +1764,19 @@
         <v>-1.65</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="V11" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="W11" s="7">
         <v>42305.75586822916</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1781,28 +1787,28 @@
         <v>11625100</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="H12" s="2">
         <v>1</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>31</v>
@@ -1810,21 +1816,21 @@
       <c r="L12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M12" s="2" t="s">
-        <v>150</v>
+      <c r="M12" s="2">
+        <v>2004</v>
       </c>
       <c r="N12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O12" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="P12" s="3" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="Q12" s="3"/>
       <c r="R12" s="3" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="S12" s="6">
         <v>-4.67</v>
@@ -1833,24 +1839,97 @@
         <v>-4.04</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="V12" s="2">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="W12" s="7">
         <v>43932.85945908564</v>
       </c>
       <c r="X12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y12" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>7466770</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M13" s="2">
+        <v>2011</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="6">
+        <v>0</v>
+      </c>
+      <c r="T13" s="6">
+        <v>0</v>
+      </c>
+      <c r="U13" s="4" t="s">
         <v>153</v>
+      </c>
+      <c r="V13" s="2">
+        <v>191</v>
+      </c>
+      <c r="W13" s="7">
+        <v>43961.64464083334</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Y65536"/>
-  <conditionalFormatting sqref="K2:K12">
+  <conditionalFormatting sqref="K2:K13">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="INCONSISTENT">
       <formula>NOT(ISERROR(SEARCH("INCONSISTENT",K2)))</formula>
     </cfRule>
@@ -1858,7 +1937,7 @@
       <formula>NOT(ISERROR(SEARCH("GENRE_OK",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L12">
+  <conditionalFormatting sqref="L2:L13">
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",L2)))</formula>
     </cfRule>
@@ -1866,12 +1945,12 @@
       <formula>NOT(ISERROR(SEARCH("ALBUM_ART",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V12">
+  <conditionalFormatting sqref="V2:V13">
     <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThanOrEqual">
       <formula>200</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X12">
+  <conditionalFormatting sqref="X2:X13">
     <cfRule type="notContainsText" dxfId="0" priority="6" operator="notContains" text="ascii">
       <formula>ISERROR(SEARCH("ascii",X2))</formula>
     </cfRule>
@@ -1882,7 +1961,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1900,19 +1979,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1926,7 +2005,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E2" s="7">
         <v>43948.67551682781</v>
@@ -1940,10 +2019,10 @@
         <v>16334985</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E3" s="7">
         <v>43873.81674494656</v>
@@ -1957,13 +2036,13 @@
         <v>24794419</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E4" s="7">
-        <v>43876.81164264229</v>
+        <v>43961.63714481935</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1974,10 +2053,10 @@
         <v>7176192</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E5" s="7">
         <v>43873.8667856177</v>
@@ -1991,10 +2070,10 @@
         <v>10332160</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E6" s="7">
         <v>43873.78914194942</v>
@@ -2008,10 +2087,10 @@
         <v>6770846</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E7" s="7">
         <v>43873.85891012724</v>
@@ -2025,10 +2104,10 @@
         <v>13749215</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E8" s="7">
         <v>43873.86218210698</v>
@@ -2042,10 +2121,10 @@
         <v>12461636</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E9" s="7">
         <v>43873.85947618695</v>
@@ -2059,13 +2138,13 @@
         <v>11625100</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E10" s="7">
-        <v>43873.81182217986</v>
+        <v>43961.63675699475</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2076,10 +2155,10 @@
         <v>5289728</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E11" s="7">
         <v>43876.78792731479</v>
@@ -2093,13 +2172,30 @@
         <v>1814528</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E12" s="7">
         <v>43876.80530935681</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>7466770</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E13" s="7">
+        <v>43961.64375412364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved ETL portion wtih postgres to new repo
</commit_message>
<xml_diff>
--- a/data/output/~media_report.xlsx
+++ b/data/output/~media_report.xlsx
@@ -1770,7 +1770,7 @@
         <v>144</v>
       </c>
       <c r="W11" s="7">
-        <v>42305.75586822916</v>
+        <v>43970.45450629989</v>
       </c>
       <c r="X11" s="3" t="s">
         <v>133</v>
@@ -1845,7 +1845,7 @@
         <v>195</v>
       </c>
       <c r="W12" s="7">
-        <v>43932.85945908564</v>
+        <v>43970.45450760752</v>
       </c>
       <c r="X12" s="3" t="s">
         <v>37</v>
@@ -1918,7 +1918,7 @@
         <v>198</v>
       </c>
       <c r="W13" s="7">
-        <v>43961.64464083334</v>
+        <v>43970.45450830195</v>
       </c>
       <c r="X13" s="3" t="s">
         <v>37</v>
@@ -2042,7 +2042,7 @@
         <v>162</v>
       </c>
       <c r="E4" s="7">
-        <v>43961.63714481935</v>
+        <v>43970.4545054895</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2144,7 +2144,7 @@
         <v>168</v>
       </c>
       <c r="E10" s="7">
-        <v>43961.63675699475</v>
+        <v>43970.45450720243</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2195,7 +2195,7 @@
         <v>171</v>
       </c>
       <c r="E13" s="7">
-        <v>43961.64375412364</v>
+        <v>43970.45450803581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tag key refactor ('artist' vs. 'artist_name', etc.)
</commit_message>
<xml_diff>
--- a/data/output/~media_report.xlsx
+++ b/data/output/~media_report.xlsx
@@ -33,16 +33,16 @@
     <t>file_ext:</t>
   </si>
   <si>
-    <t>artist:</t>
-  </si>
-  <si>
-    <t>album:</t>
-  </si>
-  <si>
-    <t>title:</t>
-  </si>
-  <si>
-    <t>track:</t>
+    <t>artist_name:</t>
+  </si>
+  <si>
+    <t>album_title:</t>
+  </si>
+  <si>
+    <t>track_title:</t>
+  </si>
+  <si>
+    <t>track_number:</t>
   </si>
   <si>
     <t>track_length:</t>
@@ -114,7 +114,7 @@
     <t>Alternative</t>
   </si>
   <si>
-    <t>ARTIST_to_GENRE_OK</t>
+    <t>GENRE_OK</t>
   </si>
   <si>
     <t>ALBUM_ART</t>
@@ -156,7 +156,7 @@
     <t>Traditional-Pop</t>
   </si>
   <si>
-    <t>INCONSISTENT_GENRE</t>
+    <t>INCONSISTENT</t>
   </si>
   <si>
     <t>2-1/2-star</t>
@@ -944,10 +944,10 @@
     <col min="5" max="5" width="38.7109375" customWidth="1"/>
     <col min="6" max="6" width="38.7109375" customWidth="1"/>
     <col min="7" max="7" width="46.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
     <col min="12" max="12" width="14.7109375" customWidth="1"/>
     <col min="13" max="13" width="5.7109375" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" customWidth="1"/>

</xml_diff>

<commit_message>
open() refactor, mkdir, and updates
</commit_message>
<xml_diff>
--- a/data/output/~media_report.xlsx
+++ b/data/output/~media_report.xlsx
@@ -1104,7 +1104,7 @@
         <v>36</v>
       </c>
       <c r="V2" s="2">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="W2" s="7">
         <v>43932.85918427083</v>
@@ -1177,7 +1177,7 @@
         <v>49</v>
       </c>
       <c r="V3" s="2">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="W3" s="7">
         <v>43876.70424291667</v>
@@ -1248,7 +1248,7 @@
         <v>58</v>
       </c>
       <c r="V4" s="2">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="W4" s="7">
         <v>43876.70372451389</v>
@@ -1325,7 +1325,7 @@
         <v>70</v>
       </c>
       <c r="V5" s="2">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="W5" s="7">
         <v>43932.85872113426</v>
@@ -1400,7 +1400,7 @@
         <v>83</v>
       </c>
       <c r="V6" s="2">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="W6" s="7">
         <v>43932.85997417824</v>
@@ -1473,7 +1473,7 @@
         <v>93</v>
       </c>
       <c r="V7" s="2">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="W7" s="7">
         <v>43876.70344572917</v>
@@ -1546,7 +1546,7 @@
         <v>102</v>
       </c>
       <c r="V8" s="2">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="W8" s="7">
         <v>43876.70200997685</v>
@@ -1621,7 +1621,7 @@
         <v>112</v>
       </c>
       <c r="V9" s="2">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="W9" s="7">
         <v>43876.78738667824</v>
@@ -1696,7 +1696,7 @@
         <v>124</v>
       </c>
       <c r="V10" s="2">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="W10" s="7">
         <v>43876.70605457176</v>
@@ -1767,7 +1767,7 @@
         <v>132</v>
       </c>
       <c r="V11" s="2">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="W11" s="7">
         <v>43970.45450629989</v>
@@ -1842,7 +1842,7 @@
         <v>142</v>
       </c>
       <c r="V12" s="2">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="W12" s="7">
         <v>43970.45450760752</v>
@@ -1915,7 +1915,7 @@
         <v>153</v>
       </c>
       <c r="V13" s="2">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="W13" s="7">
         <v>43970.45450830195</v>
@@ -2042,7 +2042,7 @@
         <v>162</v>
       </c>
       <c r="E4" s="7">
-        <v>43970.4545054895</v>
+        <v>43970.45450548951</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2093,7 +2093,7 @@
         <v>165</v>
       </c>
       <c r="E7" s="7">
-        <v>43962.69165836067</v>
+        <v>43962.69165836073</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2110,7 +2110,7 @@
         <v>166</v>
       </c>
       <c r="E8" s="7">
-        <v>43962.69165788613</v>
+        <v>43962.69165788621</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2127,7 +2127,7 @@
         <v>167</v>
       </c>
       <c r="E9" s="7">
-        <v>43962.69165755051</v>
+        <v>43962.69165755047</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2144,7 +2144,7 @@
         <v>168</v>
       </c>
       <c r="E10" s="7">
-        <v>43970.45450720243</v>
+        <v>43970.45450720222</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2161,7 +2161,7 @@
         <v>169</v>
       </c>
       <c r="E11" s="7">
-        <v>43962.69159603315</v>
+        <v>43962.69159603336</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2195,7 +2195,7 @@
         <v>171</v>
       </c>
       <c r="E13" s="7">
-        <v>43970.45450803581</v>
+        <v>43970.45450803575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>